<commit_message>
+ Added search box control; + Added order screen;
</commit_message>
<xml_diff>
--- a/Documents/Design/Final_Db_Design.xlsx
+++ b/Documents/Design/Final_Db_Design.xlsx
@@ -375,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -413,12 +413,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -439,6 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1179,7 +1193,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1328,7 @@
       <c r="G11" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="18" t="s">
         <v>3</v>
       </c>
       <c r="K11" t="s">
@@ -1348,7 +1362,7 @@
       <c r="E15" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1357,15 +1371,15 @@
         <v>21</v>
       </c>
       <c r="I16" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E17" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="17" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="E17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
@@ -1375,8 +1389,8 @@
       <c r="E18" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="16" t="s">
-        <v>49</v>
+      <c r="I18" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
@@ -1386,8 +1400,8 @@
       <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>10</v>
+      <c r="I19" s="17" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">

</xml_diff>